<commit_message>
A new level screen by Alon
</commit_message>
<xml_diff>
--- a/screens_layout/ScreensLayout.xlsx
+++ b/screens_layout/ScreensLayout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programs\Python\ScreensLayoutConverter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\BrickSmash\screens_layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD2FF1F-C172-40E6-86A7-C967D2901AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB565083-21B4-43B9-A6D7-63CAE9B6F013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Level001" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,15 @@
     <sheet name="Level009" sheetId="14" r:id="rId9"/>
     <sheet name="Level010" sheetId="15" r:id="rId10"/>
     <sheet name="Level011" sheetId="17" r:id="rId11"/>
-    <sheet name="Level Template" sheetId="5" r:id="rId12"/>
+    <sheet name="Level012" sheetId="18" r:id="rId12"/>
+    <sheet name="Level Template" sheetId="5" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="110">
   <si>
     <t>Packs:</t>
   </si>
@@ -331,6 +332,36 @@
   </si>
   <si>
     <t>c9sp4e</t>
+  </si>
+  <si>
+    <t>c1s2pe</t>
+  </si>
+  <si>
+    <t>c8s-1p2e</t>
+  </si>
+  <si>
+    <t>c1sp9e</t>
+  </si>
+  <si>
+    <t>c1s2p10e</t>
+  </si>
+  <si>
+    <t>c0sp10e</t>
+  </si>
+  <si>
+    <t>c1sp14e</t>
+  </si>
+  <si>
+    <t>c1sp17e</t>
+  </si>
+  <si>
+    <t>c1sp18e</t>
+  </si>
+  <si>
+    <t>c0sp18e</t>
+  </si>
+  <si>
+    <t>c6s4pe</t>
   </si>
 </sst>
 </file>
@@ -5433,6 +5464,1561 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7069974-7095-4233-A0E4-7EDC7466DB34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10881360" y="251460"/>
+          <a:ext cx="640210" cy="254058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>130</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{836697F2-5636-4687-8782-2949A59C084C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10881360" y="2263140"/>
+          <a:ext cx="640210" cy="254058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>130</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11EB50CC-74AE-49C5-AD79-BE70531B2261}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10881360" y="0"/>
+          <a:ext cx="640210" cy="254058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>130</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BE450B2-7631-4E7A-98A7-CCAE0296B701}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10881360" y="502920"/>
+          <a:ext cx="640210" cy="254058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>130</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEE38418-65C2-4F7A-B68B-0D5B27E544A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10881360" y="754380"/>
+          <a:ext cx="640210" cy="254058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>130</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1318FE4-C59B-416E-9EB2-6D3F966A9FBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10881360" y="1005840"/>
+          <a:ext cx="640210" cy="254058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>130</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97FF69EB-374E-4D74-9D26-8E84E2AE7BB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10881360" y="1257300"/>
+          <a:ext cx="640210" cy="254058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>130</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BB62A7D-A541-4AFA-A2A0-440C4903DDE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10881360" y="1508760"/>
+          <a:ext cx="640210" cy="254058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>130</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>2598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBC42191-9B99-4A8F-B33C-AD7BE21B9FD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10881360" y="1760220"/>
+          <a:ext cx="640210" cy="254058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>130</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35D048A9-369D-4339-AF73-0839880EB106}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10881360" y="2011680"/>
+          <a:ext cx="640210" cy="254058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>8160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D179156-48A5-480C-BD76-748DACF51193}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="7620"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08B31514-EF52-4856-906A-4D38630DD852}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="251460"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69C7C713-9BA3-4CAC-8C3B-7496869DFF4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="502920"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61F07DCF-FA5A-4F79-9F1D-0688F926C08A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="754380"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30A5C5F1-C031-4AFE-991C-CF732F8F9D28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="1005840"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFA07808-B4B2-43A0-8844-CA79F1192211}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="1257300"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63F9FF5B-CE5B-497C-AE98-67F70D8D80A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="1508760"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B2F1C31-A905-43B2-8377-A0C063A05F2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="1760220"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF85AD90-BDB7-4550-B7C4-CDC441E29BEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="2011680"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32575BB7-3DA0-4B06-BD8B-3F3E6123AE18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="2263140"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12C452DA-F820-4908-83C7-F582E2593C47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="2514600"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FE2A08F-364E-4534-8630-A32EC9920B91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="2766060"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3F70485-9CB8-457D-8DAB-32E4E9441560}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="3017520"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89921A50-FCB0-41B0-B6A4-DB0CE397D617}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="3268980"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{491D5CFD-9DC2-4E86-A31A-6895EE1C9F5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="3520440"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4E4A196-BC12-4DB9-AECB-45C929A40A46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="3771900"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEC748D0-42DA-4170-AADC-759DBEF809D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="4023360"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0358DC09-2724-491B-AE23-38910D6C99C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="4274820"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97654AFB-7F49-4507-A5C4-E9AD86D53358}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="4526280"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533940</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D28993F3-B8B2-41D8-9A10-EB1CA3400453}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="4777740"/>
+          <a:ext cx="244380" cy="252000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>2508</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EC40C95-D7BF-4C64-AFDF-2CDBD088C08C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10881360" y="2514600"/>
+          <a:ext cx="640080" cy="253968"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>130</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
         <xdr:cNvPr id="22" name="Picture 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
@@ -19704,9 +21290,9 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
@@ -19747,7 +21333,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
@@ -19778,7 +21364,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>5</v>
       </c>
@@ -19813,7 +21399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>5</v>
       </c>
@@ -19852,7 +21438,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
@@ -19893,7 +21479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -19934,7 +21520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>5</v>
       </c>
@@ -19973,7 +21559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>5</v>
       </c>
@@ -20008,7 +21594,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>2</v>
       </c>
@@ -20039,7 +21625,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>2</v>
       </c>
@@ -20072,7 +21658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -20095,7 +21681,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -20112,7 +21698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -20129,7 +21715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -20146,7 +21732,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -20163,7 +21749,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -20180,7 +21766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -20197,7 +21783,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -20214,7 +21800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -20231,7 +21817,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -20248,7 +21834,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -20292,9 +21878,9 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>15</v>
       </c>
@@ -20339,7 +21925,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -20368,7 +21954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="20" t="s">
         <v>15</v>
@@ -20397,7 +21983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
@@ -20432,7 +22018,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -20455,7 +22041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -20478,7 +22064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -20501,7 +22087,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -20524,7 +22110,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="19" t="s">
@@ -20551,7 +22137,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="19" t="s">
         <v>2</v>
@@ -20586,7 +22172,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="19" t="s">
         <v>2</v>
@@ -20621,7 +22207,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="19" t="s">
         <v>2</v>
@@ -20652,7 +22238,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="19" t="s">
         <v>11</v>
@@ -20683,7 +22269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="19" t="s">
         <v>2</v>
@@ -20714,7 +22300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="19" t="s">
@@ -20741,7 +22327,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="19" t="s">
@@ -20768,7 +22354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -20791,7 +22377,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -20814,7 +22400,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -20833,7 +22419,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="8"/>
       <c r="C20" s="5"/>
@@ -20850,7 +22436,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -20893,9 +22479,9 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="5"/>
       <c r="C1" s="23" t="s">
@@ -20930,7 +22516,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>13</v>
       </c>
@@ -20969,7 +22555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>13</v>
       </c>
@@ -21010,7 +22596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
         <v>13</v>
       </c>
@@ -21051,7 +22637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>98</v>
       </c>
@@ -21092,7 +22678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>13</v>
       </c>
@@ -21133,7 +22719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>13</v>
       </c>
@@ -21174,7 +22760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>13</v>
       </c>
@@ -21215,7 +22801,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>87</v>
       </c>
@@ -21256,7 +22842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>13</v>
       </c>
@@ -21297,7 +22883,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>13</v>
       </c>
@@ -21338,7 +22924,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>13</v>
       </c>
@@ -21373,7 +22959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="23" t="s">
         <v>13</v>
@@ -21404,7 +22990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="23" t="s">
@@ -21431,7 +23017,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -21454,7 +23040,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -21473,7 +23059,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -21490,7 +23076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -21507,7 +23093,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -21524,7 +23110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -21541,7 +23127,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -21577,16 +23163,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40A8E8E2-5591-4723-BEA0-FC4389F33B69}">
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -21617,7 +23203,623 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="M3" s="11">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="M4" s="12">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="M5" s="11">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="T5" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="M6" s="11">
+        <v>5</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="M7" s="11">
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="T7" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="M8" s="11">
+        <v>7</v>
+      </c>
+      <c r="Q8">
+        <v>7</v>
+      </c>
+      <c r="T8" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="M9" s="12">
+        <v>8</v>
+      </c>
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="T9" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="M10" s="11">
+        <v>9</v>
+      </c>
+      <c r="Q10">
+        <v>9</v>
+      </c>
+      <c r="T10" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6"/>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="M11" s="11">
+        <v>10</v>
+      </c>
+      <c r="Q11">
+        <v>10</v>
+      </c>
+      <c r="T11" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12">
+        <v>11</v>
+      </c>
+      <c r="M12" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="M13" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14">
+        <v>13</v>
+      </c>
+      <c r="M14" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15">
+        <v>14</v>
+      </c>
+      <c r="M15" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16">
+        <v>15</v>
+      </c>
+      <c r="M16" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="6"/>
+      <c r="J17">
+        <v>16</v>
+      </c>
+      <c r="M17" s="11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="6"/>
+      <c r="J18">
+        <v>17</v>
+      </c>
+      <c r="M18" s="11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19">
+        <v>18</v>
+      </c>
+      <c r="M19" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="9"/>
+      <c r="J20">
+        <v>19</v>
+      </c>
+      <c r="M20" s="12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:T21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1">
+        <v>0</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="11">
+        <v>0</v>
+      </c>
+      <c r="N1" s="10"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1">
+        <v>0</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -21640,7 +23842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -21663,7 +23865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -21686,7 +23888,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -21709,7 +23911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -21732,7 +23934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -21755,7 +23957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -21778,7 +23980,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -21801,7 +24003,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -21824,7 +24026,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -21847,7 +24049,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -21864,7 +24066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -21881,7 +24083,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -21898,7 +24100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -21915,7 +24117,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -21932,7 +24134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -21949,7 +24151,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -21966,7 +24168,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -21983,7 +24185,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -22000,7 +24202,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -22043,9 +24245,9 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -22082,7 +24284,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="20" t="s">
@@ -22113,7 +24315,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="20" t="s">
         <v>15</v>
@@ -22144,7 +24346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="20" t="s">
         <v>15</v>
@@ -22177,7 +24379,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="20" t="s">
         <v>15</v>
@@ -22208,7 +24410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="20" t="s">
@@ -22239,7 +24441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>3</v>
       </c>
@@ -22272,7 +24474,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>16</v>
       </c>
@@ -22309,7 +24511,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="19" t="s">
@@ -22340,7 +24542,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="19" t="s">
         <v>7</v>
@@ -22377,7 +24579,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -22400,7 +24602,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -22417,7 +24619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -22434,7 +24636,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -22451,7 +24653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -22468,7 +24670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -22485,7 +24687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -22502,7 +24704,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -22519,7 +24721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -22536,7 +24738,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -22553,7 +24755,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -22596,9 +24798,9 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -22629,7 +24831,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="18" t="s">
@@ -22656,7 +24858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="18" t="s">
         <v>5</v>
@@ -22687,7 +24889,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>5</v>
       </c>
@@ -22722,7 +24924,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
@@ -22757,7 +24959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="18" t="s">
         <v>30</v>
@@ -22788,7 +24990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="18" t="s">
@@ -22815,7 +25017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -22838,7 +25040,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -22861,7 +25063,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -22884,7 +25086,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -22907,7 +25109,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>13</v>
       </c>
@@ -22926,7 +25128,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>3</v>
       </c>
@@ -22947,7 +25149,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>24</v>
       </c>
@@ -22970,7 +25172,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>18</v>
       </c>
@@ -22995,7 +25197,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
         <v>25</v>
       </c>
@@ -23022,7 +25224,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>5</v>
       </c>
@@ -23051,7 +25253,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>26</v>
       </c>
@@ -23082,7 +25284,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>15</v>
       </c>
@@ -23115,7 +25317,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -23132,7 +25334,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -23175,9 +25377,9 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="20" t="s">
@@ -23216,7 +25418,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="20" t="s">
         <v>15</v>
@@ -23251,7 +25453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="20" t="s">
         <v>15</v>
@@ -23288,7 +25490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="20" t="s">
         <v>42</v>
@@ -23325,7 +25527,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="24" t="s">
@@ -23358,7 +25560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="24" t="s">
@@ -23391,7 +25593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="20" t="s">
         <v>15</v>
@@ -23428,7 +25630,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="20" t="s">
         <v>15</v>
@@ -23465,7 +25667,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>3</v>
       </c>
@@ -23504,7 +25706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>3</v>
       </c>
@@ -23539,7 +25741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>3</v>
       </c>
@@ -23568,7 +25770,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="15" t="s">
         <v>39</v>
@@ -23589,7 +25791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="15" t="s">
         <v>3</v>
@@ -23614,7 +25816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="15" t="s">
         <v>3</v>
@@ -23637,7 +25839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>3</v>
       </c>
@@ -23660,7 +25862,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>3</v>
       </c>
@@ -23681,7 +25883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>3</v>
       </c>
@@ -23704,7 +25906,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>18</v>
       </c>
@@ -23727,7 +25929,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -23744,7 +25946,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -23761,7 +25963,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -23805,9 +26007,9 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>13</v>
       </c>
@@ -23850,7 +26052,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>13</v>
       </c>
@@ -23885,7 +26087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>13</v>
       </c>
@@ -23922,7 +26124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
         <v>13</v>
       </c>
@@ -23961,7 +26163,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>26</v>
       </c>
@@ -24002,7 +26204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
@@ -24043,7 +26245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>33</v>
       </c>
@@ -24084,7 +26286,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="14" t="s">
         <v>26</v>
@@ -24121,7 +26323,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="14" t="s">
         <v>48</v>
@@ -24158,7 +26360,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="14" t="s">
         <v>26</v>
@@ -24195,7 +26397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="14" t="s">
@@ -24228,7 +26430,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="14" t="s">
@@ -24255,7 +26457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -24278,7 +26480,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="17" t="s">
         <v>18</v>
@@ -24305,7 +26507,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="17" t="s">
         <v>18</v>
@@ -24328,7 +26530,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>18</v>
       </c>
@@ -24357,7 +26559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -24374,7 +26576,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -24391,7 +26593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -24408,7 +26610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -24425,7 +26627,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -24468,9 +26670,9 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="19" t="s">
@@ -24511,7 +26713,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="19" t="s">
         <v>2</v>
@@ -24548,7 +26750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
@@ -24589,7 +26791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>60</v>
       </c>
@@ -24630,7 +26832,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>2</v>
       </c>
@@ -24671,7 +26873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>2</v>
       </c>
@@ -24712,7 +26914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>2</v>
       </c>
@@ -24753,7 +26955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -24794,7 +26996,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>2</v>
       </c>
@@ -24835,7 +27037,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>27</v>
       </c>
@@ -24876,7 +27078,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>2</v>
       </c>
@@ -24917,7 +27119,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
         <v>7</v>
       </c>
@@ -24952,7 +27154,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>2</v>
       </c>
@@ -24987,7 +27189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>2</v>
       </c>
@@ -25014,7 +27216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -25031,7 +27233,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -25048,7 +27250,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -25065,7 +27267,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -25082,7 +27284,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -25099,7 +27301,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -25116,7 +27318,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -25159,9 +27361,9 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
@@ -25202,7 +27404,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>26</v>
       </c>
@@ -25243,7 +27445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>53</v>
       </c>
@@ -25284,7 +27486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>5</v>
       </c>
@@ -25325,7 +27527,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
@@ -25366,7 +27568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -25407,7 +27609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="16" t="s">
         <v>67</v>
@@ -25438,7 +27640,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -25461,7 +27663,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -25484,7 +27686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -25507,7 +27709,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="24" t="s">
         <v>19</v>
@@ -25538,7 +27740,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="21" t="s">
         <v>63</v>
@@ -25563,7 +27765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="23" t="s">
         <v>13</v>
@@ -25588,7 +27790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="20" t="s">
         <v>15</v>
@@ -25613,7 +27815,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>65</v>
       </c>
@@ -25640,7 +27842,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
         <v>13</v>
       </c>
@@ -25667,7 +27869,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>45</v>
       </c>
@@ -25694,7 +27896,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
         <v>19</v>
       </c>
@@ -25721,7 +27923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -25738,7 +27940,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -25755,7 +27957,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -25798,9 +28000,9 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="16" t="s">
@@ -25841,7 +28043,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="16" t="s">
@@ -25874,7 +28076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="16" t="s">
@@ -25905,7 +28107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="14" t="s">
@@ -25936,7 +28138,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="14" t="s">
@@ -25969,7 +28171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -25992,7 +28194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -26015,7 +28217,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -26038,7 +28240,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -26063,7 +28265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -26092,7 +28294,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="20" t="s">
@@ -26125,7 +28327,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -26148,7 +28350,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -26171,7 +28373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -26194,7 +28396,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -26217,7 +28419,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -26240,7 +28442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -26257,7 +28459,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -26274,7 +28476,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -26291,7 +28493,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -26308,7 +28510,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -26352,9 +28554,9 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -26391,7 +28593,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="19" t="s">
@@ -26424,7 +28626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="19" t="s">
@@ -26457,7 +28659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="19" t="s">
@@ -26490,7 +28692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="19" t="s">
@@ -26523,7 +28725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -26552,7 +28754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -26577,7 +28779,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -26604,7 +28806,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -26633,7 +28835,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -26662,7 +28864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -26689,7 +28891,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>3</v>
       </c>
@@ -26712,7 +28914,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>3</v>
       </c>
@@ -26737,7 +28939,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="15" t="s">
         <v>3</v>
@@ -26758,7 +28960,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="15" t="s">
@@ -26777,7 +28979,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="15" t="s">
@@ -26796,7 +28998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="15" t="s">
         <v>3</v>
@@ -26815,7 +29017,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="15" t="s">
         <v>3</v>
@@ -26834,7 +29036,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>3</v>
       </c>
@@ -26853,7 +29055,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>3</v>
       </c>
@@ -26872,7 +29074,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>

</xml_diff>